<commit_message>
Added codes for heart failure and MS to the codes and removed hypercholesterolemia
</commit_message>
<xml_diff>
--- a/codes_validation.xlsx
+++ b/codes_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maestro/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maestro/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F567F5DA-50F9-D744-B1B5-A623F02B3383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21670151-87F0-BE4C-A033-455372F1B8A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41480" yWindow="2860" windowWidth="27640" windowHeight="16940" xr2:uid="{91475830-1A13-0A48-97DD-FE5860C8D75F}"/>
+    <workbookView xWindow="39560" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{91475830-1A13-0A48-97DD-FE5860C8D75F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
   <si>
     <t>I12</t>
   </si>
@@ -236,37 +236,46 @@
     <t>Other hypothyroidism</t>
   </si>
   <si>
-    <t>E780</t>
-  </si>
-  <si>
-    <t>hyperchol</t>
-  </si>
-  <si>
-    <t>pure hypercholesterolemia</t>
-  </si>
-  <si>
-    <t>E782</t>
-  </si>
-  <si>
-    <t>mixed hypercholesterolemia</t>
-  </si>
-  <si>
-    <t>E785</t>
-  </si>
-  <si>
-    <t>hyperlipidaemia</t>
-  </si>
-  <si>
-    <t>E788</t>
-  </si>
-  <si>
-    <t>E789</t>
-  </si>
-  <si>
-    <t>Other disorders of lipoprotein metabolism</t>
-  </si>
-  <si>
-    <t>Dirorder of lipoprotein metabolism</t>
+    <t>I50</t>
+  </si>
+  <si>
+    <t>I110</t>
+  </si>
+  <si>
+    <t>I130</t>
+  </si>
+  <si>
+    <t>I42</t>
+  </si>
+  <si>
+    <t>hf</t>
+  </si>
+  <si>
+    <t>heart failure</t>
+  </si>
+  <si>
+    <t>HTN heart disease with CHF</t>
+  </si>
+  <si>
+    <t>HTN heart and renal disease with CHF</t>
+  </si>
+  <si>
+    <t>HTN with heart and renal disease with both CKD and CHF</t>
+  </si>
+  <si>
+    <t>Cardiomyopathies</t>
+  </si>
+  <si>
+    <t>I132</t>
+  </si>
+  <si>
+    <t>G35</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Multiple Sclerosis</t>
   </si>
 </sst>
 </file>
@@ -632,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C27780-0A00-2841-8EE0-8E19706826C1}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,54 +1009,65 @@
         <v>67</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>